<commit_message>
Added Registration Page and Refactored code.
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gowri\workspace\Yahoo\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gowri\workspace\Yahoo\Yahoo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="10381" windowWidth="25135" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" windowHeight="10381" windowWidth="25135" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
     <sheet name="LoginDetails" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Registration" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>selenium</t>
   </si>
@@ -67,6 +67,12 @@
   <si>
     <t xml:space="preserve">bXFxOTg3NjU0bXFxOTg3NjU0
 </t>
+  </si>
+  <si>
+    <t>Gowri</t>
+  </si>
+  <si>
+    <t>Kumar</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -555,12 +561,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Code in egistration File and Updted config file with Selecting dropdown list function,
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>selenium</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Kumar</t>
+  </si>
+  <si>
+    <t>tapanagkumar98499</t>
+  </si>
+  <si>
+    <t>Yahoo_1234</t>
   </si>
 </sst>
 </file>
@@ -80,7 +86,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +98,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,17 +128,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,20 +578,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>